<commit_message>
fw update - basic functionality complete
</commit_message>
<xml_diff>
--- a/pins.xlsx
+++ b/pins.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shuri\Dropbox\Robotics\github\motor-driver\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kirillov\Dropbox\Robotics\github\motor-driver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8359B4D4-11A0-4096-B51E-F9F6E2316F00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{2592871D-5CB4-45BA-AF33-93636A88B9F2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416"/>
   </bookViews>
   <sheets>
     <sheet name="V1.1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -102,9 +101,6 @@
     <t>JMP1</t>
   </si>
   <si>
-    <t>M2_FLAG</t>
-  </si>
-  <si>
     <t>ENC2_B</t>
   </si>
   <si>
@@ -117,12 +113,6 @@
     <t>ENC1_A</t>
   </si>
   <si>
-    <t>M1_FLAG</t>
-  </si>
-  <si>
-    <t>ENABLE</t>
-  </si>
-  <si>
     <t>M1_DIR</t>
   </si>
   <si>
@@ -174,13 +164,22 @@
     <t>Error status flag for driver2</t>
   </si>
   <si>
-    <t>Enables both motor drivers</t>
+    <t>DISABLE</t>
+  </si>
+  <si>
+    <t>Disables both motor drivers</t>
+  </si>
+  <si>
+    <t>M2_ERROR</t>
+  </si>
+  <si>
+    <t>M1_ERROR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -271,13 +270,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -591,33 +590,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8072886-2C49-4894-A38C-F89DAA42CA1F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.08984375" customWidth="1"/>
-    <col min="2" max="2" width="15.08984375" customWidth="1"/>
+    <col min="1" max="1" width="8.109375" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-    </row>
-    <row r="2" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+    </row>
+    <row r="2" spans="1:4" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -628,34 +627,34 @@
         <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -665,19 +664,19 @@
       </c>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -686,10 +685,10 @@
         <v>21</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
@@ -698,126 +697,126 @@
         <v>22</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="4" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="8" t="s">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D15" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D18" s="3"/>
     </row>

</xml_diff>